<commit_message>
Fix typo in sheet
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/aj_yu_mail_utoronto_ca/Documents/MSc/Research/git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanyu\Documents\MSc\Research\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13A13A5F-31DB-4800-823B-10064DBBFD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A2DB0B-7DD5-46CE-9B11-3F3107BF95DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="19260" windowHeight="15405" xr2:uid="{ADE5AF9D-5035-41AC-9350-6A444D7E7345}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ADE5AF9D-5035-41AC-9350-6A444D7E7345}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter testing" sheetId="3" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -85,9 +83,6 @@
     <t>Initial upper plate extent</t>
   </si>
   <si>
-    <t>Initial strain extent</t>
-  </si>
-  <si>
     <t>0.5-1.5</t>
   </si>
   <si>
@@ -103,9 +98,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>Geotherm (MOHO temp)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Whole litho </t>
   </si>
   <si>
@@ -115,9 +107,6 @@
     <t>Crust only</t>
   </si>
   <si>
-    <t>Deformed layer(s)</t>
-  </si>
-  <si>
     <t>°</t>
   </si>
   <si>
@@ -178,9 +167,6 @@
     <t>z</t>
   </si>
   <si>
-    <t>Total model</t>
-  </si>
-  <si>
     <t>Ref (881)</t>
   </si>
   <si>
@@ -209,6 +195,18 @@
   </si>
   <si>
     <t>5+4</t>
+  </si>
+  <si>
+    <t>Total # of models</t>
+  </si>
+  <si>
+    <t>Preferentially deformed layer(s)</t>
+  </si>
+  <si>
+    <t>Initial geotherm (MOHO temp)</t>
+  </si>
+  <si>
+    <t>Initial plastic strain extent</t>
   </si>
 </sst>
 </file>
@@ -429,9 +427,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,7 +467,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -575,7 +573,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -717,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -728,24 +726,24 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="11" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -756,15 +754,15 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D2" s="10">
         <v>0.1</v>
@@ -794,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="22"/>
       <c r="C3" s="5"/>
@@ -826,12 +824,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10">
         <v>6</v>
@@ -857,49 +855,49 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="22"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="H5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="10">
         <v>3</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -907,15 +905,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="22"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>4</v>
@@ -926,24 +924,24 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="12">
         <v>3</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -951,15 +949,15 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="23"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>0</v>
@@ -970,12 +968,12 @@
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -984,28 +982,28 @@
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="22"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1013,9 +1011,9 @@
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>13</v>
@@ -1038,7 +1036,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="22"/>
       <c r="C13" s="5"/>
@@ -1057,7 +1055,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -1082,7 +1080,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="22"/>
       <c r="C15" s="5"/>
@@ -1101,7 +1099,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1124,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="20"/>
       <c r="C17" s="5"/>
@@ -1145,7 +1143,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1158,13 +1156,13 @@
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1173,9 +1171,9 @@
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <f>30+4+10+10+10+10+10+10</f>
@@ -1196,42 +1194,42 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1256,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1285,7 +1283,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1310,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1336,10 +1334,10 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1363,7 +1361,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1387,7 +1385,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1414,7 +1412,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1438,9 +1436,9 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1457,13 +1455,13 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="28"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="28"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -1471,7 +1469,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>5</v>
@@ -1483,18 +1481,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="27">
         <v>273</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="24">
         <v>0</v>
@@ -1503,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <f>A2 + (D3/B3*E3)-(C3*E3*E3)/(2*B3)</f>
         <v>633</v>
@@ -1525,7 +1523,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <f>A3 + (D4/B4*E4)-(C4*E4*E4)/(2*B4)</f>
         <v>881</v>
@@ -1547,7 +1545,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f t="shared" ref="A5" si="0">A4 + (D5/B5*E5)-(C5*E5*E5)/(2*B5)</f>
         <v>1579.6666666666667</v>
@@ -1569,7 +1567,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>A5+(D6/B6)*E6</f>
         <v>1793</v>
@@ -1591,7 +1589,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="18" s="28" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>